<commit_message>
add menu display option
</commit_message>
<xml_diff>
--- a/workspaces/msk/src/configs/menu/list.xlsx
+++ b/workspaces/msk/src/configs/menu/list.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\Practice\Latihan Proyek\Proyek\menu-simple-kit\workspaces\msk\src\configs\menu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49897879-6C42-4F22-9219-F2832C8F1AAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616A7AB3-F1D8-4DA2-95AD-9E63D25B8C35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="20490" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Food" sheetId="1" r:id="rId1"/>
-    <sheet name="Drink" sheetId="2" r:id="rId2"/>
-    <sheet name="Snack" sheetId="3" r:id="rId3"/>
-    <sheet name="Promo" sheetId="4" r:id="rId4"/>
+    <sheet name="Promo" sheetId="4" r:id="rId1"/>
+    <sheet name="Food" sheetId="1" r:id="rId2"/>
+    <sheet name="Drink" sheetId="2" r:id="rId3"/>
+    <sheet name="Snack" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -482,6 +482,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1:E2" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -489,14 +530,14 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25.125" customWidth="1"/>
     <col min="3" max="3" width="51.75" customWidth="1"/>
     <col min="4" max="4" width="9.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -513,7 +554,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -530,7 +571,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -589,19 +630,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.25" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -618,7 +659,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -635,7 +676,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -660,15 +701,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -685,7 +726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -700,47 +741,6 @@
       </c>
       <c r="E2" t="s">
         <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="A1:E2" numberStoredAsText="1"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>